<commit_message>
towards getting time series structure achieved
</commit_message>
<xml_diff>
--- a/data/Input_data_TS.xlsx
+++ b/data/Input_data_TS.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustintharper/Documents/R/Utah/boron/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB7162A-F6F0-DB47-B5E6-C12964A3B94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6709E9-8620-604D-A55B-B41772CFB8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="2840" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7800" yWindow="2840" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="proxy" sheetId="1" r:id="rId1"/>
     <sheet name="proxy2" sheetId="2" r:id="rId2"/>
+    <sheet name="proxy3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="7">
   <si>
     <t>d11B</t>
   </si>
@@ -1879,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA73E470-5C8A-DE47-BF69-B9D777964055}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1929,9 +1930,6 @@
       <c r="A3">
         <v>58.621000000000002</v>
       </c>
-      <c r="C3">
-        <v>0.15</v>
-      </c>
       <c r="D3">
         <v>-1.1299999999999999</v>
       </c>
@@ -1946,9 +1944,6 @@
       <c r="A4">
         <v>58.441000000000003</v>
       </c>
-      <c r="C4">
-        <v>0.13</v>
-      </c>
       <c r="D4">
         <v>-1.22</v>
       </c>
@@ -1963,9 +1958,6 @@
       <c r="A5">
         <v>58.286000000000001</v>
       </c>
-      <c r="C5">
-        <v>0.115</v>
-      </c>
       <c r="D5">
         <v>-1.07</v>
       </c>
@@ -1980,9 +1972,6 @@
       <c r="A6">
         <v>58.133000000000003</v>
       </c>
-      <c r="C6">
-        <v>0.215</v>
-      </c>
       <c r="D6">
         <v>-1.3</v>
       </c>
@@ -1997,9 +1986,6 @@
       <c r="A7">
         <v>58.101999999999997</v>
       </c>
-      <c r="C7">
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="D7">
         <v>-1.59</v>
       </c>
@@ -2048,9 +2034,6 @@
       <c r="A10">
         <v>58.085999999999999</v>
       </c>
-      <c r="C10">
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="E10">
         <v>4.33</v>
       </c>
@@ -2062,9 +2045,6 @@
       <c r="A11">
         <v>58.085999999999999</v>
       </c>
-      <c r="C11">
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="E11">
         <v>4.47</v>
       </c>
@@ -2076,9 +2056,6 @@
       <c r="A12">
         <v>58.081000000000003</v>
       </c>
-      <c r="C12">
-        <v>0.1</v>
-      </c>
       <c r="E12">
         <v>4.57</v>
       </c>
@@ -2090,9 +2067,6 @@
       <c r="A13">
         <v>58.067999999999998</v>
       </c>
-      <c r="C13">
-        <v>0.115</v>
-      </c>
       <c r="E13">
         <v>4.34</v>
       </c>
@@ -2104,9 +2078,6 @@
       <c r="A14">
         <v>58.064</v>
       </c>
-      <c r="C14">
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="D14">
         <v>-1.51</v>
       </c>
@@ -2121,9 +2092,6 @@
       <c r="A15">
         <v>58.045000000000002</v>
       </c>
-      <c r="C15">
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="D15">
         <v>-1.62</v>
       </c>
@@ -2178,9 +2146,6 @@
       <c r="A18">
         <v>57.619</v>
       </c>
-      <c r="C18">
-        <v>0.16500000000000001</v>
-      </c>
       <c r="D18">
         <v>-1.6</v>
       </c>
@@ -2195,9 +2160,6 @@
       <c r="A19">
         <v>57.5</v>
       </c>
-      <c r="C19">
-        <v>0.15</v>
-      </c>
       <c r="D19">
         <v>-1.32</v>
       </c>
@@ -2212,9 +2174,6 @@
       <c r="A20">
         <v>57.338000000000001</v>
       </c>
-      <c r="C20">
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="D20">
         <v>-1.62</v>
       </c>
@@ -2229,9 +2188,6 @@
       <c r="A21">
         <v>57.225999999999999</v>
       </c>
-      <c r="C21">
-        <v>0.13</v>
-      </c>
       <c r="D21">
         <v>-1.29</v>
       </c>
@@ -2246,9 +2202,6 @@
       <c r="A22">
         <v>57.073999999999998</v>
       </c>
-      <c r="C22">
-        <v>0.125</v>
-      </c>
       <c r="D22">
         <v>-1.42</v>
       </c>
@@ -2263,9 +2216,6 @@
       <c r="A23">
         <v>56.12</v>
       </c>
-      <c r="C23">
-        <v>0.13</v>
-      </c>
       <c r="D23">
         <v>-1.18</v>
       </c>
@@ -2280,9 +2230,6 @@
       <c r="A24">
         <v>56.12</v>
       </c>
-      <c r="C24">
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="D24">
         <v>-1.18</v>
       </c>
@@ -2354,9 +2301,6 @@
       <c r="A28">
         <v>55.957000000000001</v>
       </c>
-      <c r="C28">
-        <v>0.22500000000000001</v>
-      </c>
       <c r="D28">
         <v>-1.45</v>
       </c>
@@ -2411,9 +2355,6 @@
       <c r="A31">
         <v>55.945999999999998</v>
       </c>
-      <c r="C31">
-        <v>0.15</v>
-      </c>
       <c r="D31">
         <v>-1.62</v>
       </c>
@@ -2428,9 +2369,6 @@
       <c r="A32">
         <v>55.933999999999997</v>
       </c>
-      <c r="C32">
-        <v>0.2</v>
-      </c>
       <c r="D32">
         <v>-2</v>
       </c>
@@ -2445,9 +2383,6 @@
       <c r="A33">
         <v>55.932000000000002</v>
       </c>
-      <c r="C33">
-        <v>0.17</v>
-      </c>
       <c r="D33">
         <v>-1.99</v>
       </c>
@@ -2462,9 +2397,6 @@
       <c r="A34">
         <v>55.932000000000002</v>
       </c>
-      <c r="C34">
-        <v>0.115</v>
-      </c>
       <c r="D34">
         <v>-1.99</v>
       </c>
@@ -2539,9 +2471,6 @@
       <c r="A38">
         <v>55.901000000000003</v>
       </c>
-      <c r="C38">
-        <v>0.105</v>
-      </c>
       <c r="D38">
         <v>-1.81</v>
       </c>
@@ -2556,9 +2485,6 @@
       <c r="A39">
         <v>55.887999999999998</v>
       </c>
-      <c r="C39">
-        <v>0.115</v>
-      </c>
       <c r="D39">
         <v>-1.75</v>
       </c>
@@ -2613,9 +2539,6 @@
       <c r="A42">
         <v>55.845999999999997</v>
       </c>
-      <c r="C42">
-        <v>0.14499999999999999</v>
-      </c>
       <c r="D42">
         <v>-1.51</v>
       </c>
@@ -2630,9 +2553,6 @@
       <c r="A43">
         <v>55.814999999999998</v>
       </c>
-      <c r="C43">
-        <v>0.115</v>
-      </c>
       <c r="D43">
         <v>-1.49</v>
       </c>
@@ -2647,9 +2567,6 @@
       <c r="A44">
         <v>55.795999999999999</v>
       </c>
-      <c r="C44">
-        <v>0.19</v>
-      </c>
       <c r="D44">
         <v>-1.45</v>
       </c>
@@ -2664,9 +2581,6 @@
       <c r="A45">
         <v>55.787999999999997</v>
       </c>
-      <c r="C45">
-        <v>0.115</v>
-      </c>
       <c r="D45">
         <v>-1.57</v>
       </c>
@@ -2681,9 +2595,6 @@
       <c r="A46">
         <v>55.738999999999997</v>
       </c>
-      <c r="C46">
-        <v>9.5000000000000001E-2</v>
-      </c>
       <c r="E46">
         <v>3.84</v>
       </c>
@@ -2748,6 +2659,679 @@
         <v>3.62</v>
       </c>
       <c r="F49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C29353F-7B00-6644-95B0-3980AAFDD8F9}">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>58.776000000000003</v>
+      </c>
+      <c r="B2">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="C2">
+        <v>0.13</v>
+      </c>
+      <c r="D2">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="E2">
+        <v>3.59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>58.621000000000002</v>
+      </c>
+      <c r="D3">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="E3">
+        <v>3.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>58.441000000000003</v>
+      </c>
+      <c r="D4">
+        <v>-1.22</v>
+      </c>
+      <c r="E4">
+        <v>3.98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>58.286000000000001</v>
+      </c>
+      <c r="D5">
+        <v>-1.07</v>
+      </c>
+      <c r="E5">
+        <v>3.82</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>58.133000000000003</v>
+      </c>
+      <c r="D6">
+        <v>-1.3</v>
+      </c>
+      <c r="E6">
+        <v>3.93</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>58.101999999999997</v>
+      </c>
+      <c r="D7">
+        <v>-1.59</v>
+      </c>
+      <c r="E7">
+        <v>4.37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>58.100999999999999</v>
+      </c>
+      <c r="B8">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="C8">
+        <v>0.115</v>
+      </c>
+      <c r="E8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>58.098999999999997</v>
+      </c>
+      <c r="B9">
+        <v>16.22</v>
+      </c>
+      <c r="C9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E9">
+        <v>4.16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>58.085999999999999</v>
+      </c>
+      <c r="E10">
+        <v>4.47</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>57.987000000000002</v>
+      </c>
+      <c r="B11">
+        <v>16.47</v>
+      </c>
+      <c r="C11">
+        <v>0.13</v>
+      </c>
+      <c r="D11">
+        <v>-1.65</v>
+      </c>
+      <c r="E11">
+        <v>3.88</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>57.805999999999997</v>
+      </c>
+      <c r="B12">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="C12">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D12">
+        <v>-1.53</v>
+      </c>
+      <c r="E12">
+        <v>3.52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>57.619</v>
+      </c>
+      <c r="D13">
+        <v>-1.6</v>
+      </c>
+      <c r="E13">
+        <v>3.89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>57.5</v>
+      </c>
+      <c r="D14">
+        <v>-1.32</v>
+      </c>
+      <c r="E14">
+        <v>3.38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>57.338000000000001</v>
+      </c>
+      <c r="D15">
+        <v>-1.62</v>
+      </c>
+      <c r="E15">
+        <v>3.67</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>57.225999999999999</v>
+      </c>
+      <c r="E16">
+        <v>3.58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>57.073999999999998</v>
+      </c>
+      <c r="D17">
+        <v>-1.42</v>
+      </c>
+      <c r="E17">
+        <v>3.77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>56.12</v>
+      </c>
+      <c r="E18">
+        <v>3.63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>55.965000000000003</v>
+      </c>
+      <c r="B19">
+        <v>15.76</v>
+      </c>
+      <c r="C19">
+        <v>0.215</v>
+      </c>
+      <c r="D19">
+        <v>-1.35</v>
+      </c>
+      <c r="E19">
+        <v>3.9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>55.957000000000001</v>
+      </c>
+      <c r="D20">
+        <v>-1.45</v>
+      </c>
+      <c r="E20">
+        <v>3.53</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>55.956000000000003</v>
+      </c>
+      <c r="B21">
+        <v>15.46</v>
+      </c>
+      <c r="C21">
+        <v>0.11</v>
+      </c>
+      <c r="D21">
+        <v>-1.55</v>
+      </c>
+      <c r="E21">
+        <v>3.54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>55.95</v>
+      </c>
+      <c r="B22">
+        <v>15.73</v>
+      </c>
+      <c r="C22">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="D22">
+        <v>-1.53</v>
+      </c>
+      <c r="E22">
+        <v>3.33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>55.945999999999998</v>
+      </c>
+      <c r="D23">
+        <v>-1.62</v>
+      </c>
+      <c r="E23">
+        <v>3.35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>55.933999999999997</v>
+      </c>
+      <c r="D24">
+        <v>-2</v>
+      </c>
+      <c r="E24">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>55.932000000000002</v>
+      </c>
+      <c r="D25">
+        <v>-1.99</v>
+      </c>
+      <c r="E25">
+        <v>5.04</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>55.932000000000002</v>
+      </c>
+      <c r="D26">
+        <v>-1.99</v>
+      </c>
+      <c r="E26">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>55.927</v>
+      </c>
+      <c r="B27">
+        <v>14.82</v>
+      </c>
+      <c r="C27">
+        <v>0.15</v>
+      </c>
+      <c r="D27">
+        <v>-2</v>
+      </c>
+      <c r="E27">
+        <v>5.37</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>55.914000000000001</v>
+      </c>
+      <c r="B28">
+        <v>15.11</v>
+      </c>
+      <c r="C28">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D28">
+        <v>-1.89</v>
+      </c>
+      <c r="E28">
+        <v>5.09</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>55.901000000000003</v>
+      </c>
+      <c r="B29">
+        <v>14.45</v>
+      </c>
+      <c r="C29">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="D29">
+        <v>-1.81</v>
+      </c>
+      <c r="E29">
+        <v>4.83</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>55.901000000000003</v>
+      </c>
+      <c r="D30">
+        <v>-1.81</v>
+      </c>
+      <c r="E30">
+        <v>4.83</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>55.887999999999998</v>
+      </c>
+      <c r="D31">
+        <v>-1.75</v>
+      </c>
+      <c r="E31">
+        <v>5.01</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>55.884999999999998</v>
+      </c>
+      <c r="B32">
+        <v>14.9</v>
+      </c>
+      <c r="C32">
+        <v>0.15</v>
+      </c>
+      <c r="D32">
+        <v>-1.84</v>
+      </c>
+      <c r="E32">
+        <v>4.41</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>55.872</v>
+      </c>
+      <c r="B33">
+        <v>15.09</v>
+      </c>
+      <c r="C33">
+        <v>0.12</v>
+      </c>
+      <c r="D33">
+        <v>-1.57</v>
+      </c>
+      <c r="E33">
+        <v>4.79</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>55.845999999999997</v>
+      </c>
+      <c r="D34">
+        <v>-1.51</v>
+      </c>
+      <c r="E34">
+        <v>4.08</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>55.814999999999998</v>
+      </c>
+      <c r="D35">
+        <v>-1.49</v>
+      </c>
+      <c r="E35">
+        <v>3.83</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>55.795999999999999</v>
+      </c>
+      <c r="D36">
+        <v>-1.45</v>
+      </c>
+      <c r="E36">
+        <v>4.08</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>55.787999999999997</v>
+      </c>
+      <c r="D37">
+        <v>-1.57</v>
+      </c>
+      <c r="E37">
+        <v>3.98</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>55.738999999999997</v>
+      </c>
+      <c r="E38">
+        <v>3.84</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>55.715000000000003</v>
+      </c>
+      <c r="B39">
+        <v>15.39</v>
+      </c>
+      <c r="C39">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D39">
+        <v>-1.65</v>
+      </c>
+      <c r="E39">
+        <v>4.3</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>55.71</v>
+      </c>
+      <c r="B40">
+        <v>15.4</v>
+      </c>
+      <c r="C40">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="D40">
+        <v>-1.67</v>
+      </c>
+      <c r="E40">
+        <v>3.65</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>55.45</v>
+      </c>
+      <c r="B41">
+        <v>15.22</v>
+      </c>
+      <c r="C41">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="D41">
+        <v>-1.6</v>
+      </c>
+      <c r="E41">
+        <v>3.62</v>
+      </c>
+      <c r="F41" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pH + dic paramater-based model added, fixed relative change terms in pco2 + dic paramter-based model and it's running
</commit_message>
<xml_diff>
--- a/data/Input_data_TS.xlsx
+++ b/data/Input_data_TS.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustintharper/Documents/R/Utah/boron/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6709E9-8620-604D-A55B-B41772CFB8DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E261F1A-3D92-2C40-A3B1-A590E4DF0E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="2840" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7800" yWindow="2840" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="proxy" sheetId="1" r:id="rId1"/>
     <sheet name="proxy2" sheetId="2" r:id="rId2"/>
     <sheet name="proxy3" sheetId="3" r:id="rId3"/>
+    <sheet name="proxy4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="7">
   <si>
     <t>d11B</t>
   </si>
@@ -2671,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C29353F-7B00-6644-95B0-3980AAFDD8F9}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3338,4 +3339,233 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E3B8CC-8407-8C4C-BFA2-F0515436463B}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>58.776000000000003</v>
+      </c>
+      <c r="B2">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="C2">
+        <v>0.13</v>
+      </c>
+      <c r="D2">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="E2">
+        <v>3.59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>58.621000000000002</v>
+      </c>
+      <c r="D3">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="E3">
+        <v>3.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>58.101999999999997</v>
+      </c>
+      <c r="D4">
+        <v>-1.59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>58.100999999999999</v>
+      </c>
+      <c r="B5">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.115</v>
+      </c>
+      <c r="E5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>58.085999999999999</v>
+      </c>
+      <c r="E6">
+        <v>4.47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>57.987000000000002</v>
+      </c>
+      <c r="B7">
+        <v>16.47</v>
+      </c>
+      <c r="C7">
+        <v>0.13</v>
+      </c>
+      <c r="D7">
+        <v>-1.65</v>
+      </c>
+      <c r="E7">
+        <v>3.88</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>57.225999999999999</v>
+      </c>
+      <c r="E8">
+        <v>3.58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>57.073999999999998</v>
+      </c>
+      <c r="D9">
+        <v>-1.42</v>
+      </c>
+      <c r="E9">
+        <v>3.77</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>55.95</v>
+      </c>
+      <c r="B10">
+        <v>15.73</v>
+      </c>
+      <c r="C10">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="D10">
+        <v>-1.53</v>
+      </c>
+      <c r="E10">
+        <v>3.33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>55.932000000000002</v>
+      </c>
+      <c r="D11">
+        <v>-1.99</v>
+      </c>
+      <c r="E11">
+        <v>5.04</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>55.884999999999998</v>
+      </c>
+      <c r="B12">
+        <v>14.9</v>
+      </c>
+      <c r="C12">
+        <v>0.15</v>
+      </c>
+      <c r="D12">
+        <v>-1.84</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>55.787999999999997</v>
+      </c>
+      <c r="D13">
+        <v>-1.57</v>
+      </c>
+      <c r="E13">
+        <v>3.98</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>55.738999999999997</v>
+      </c>
+      <c r="E14">
+        <v>3.84</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
time series model (including multispecies d11B vitals) inversion running, and with dic+pco2 and dic+pH options
</commit_message>
<xml_diff>
--- a/data/Input_data_TS.xlsx
+++ b/data/Input_data_TS.xlsx
@@ -8,22 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dustintharper/Documents/R/Utah/boron/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E261F1A-3D92-2C40-A3B1-A590E4DF0E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583AD844-774F-054B-B4A6-472616E00AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="2840" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7800" yWindow="2840" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="proxy" sheetId="1" r:id="rId1"/>
     <sheet name="proxy2" sheetId="2" r:id="rId2"/>
     <sheet name="proxy3" sheetId="3" r:id="rId3"/>
     <sheet name="proxy4" sheetId="4" r:id="rId4"/>
+    <sheet name="proxy5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="8">
   <si>
     <t>d11B</t>
   </si>
@@ -45,11 +58,17 @@
   <si>
     <t>d11Bsd</t>
   </si>
+  <si>
+    <t>Tsac</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -186,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +385,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -527,8 +552,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -886,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F49"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1849,7 +1878,7 @@
         <v>3.65</v>
       </c>
       <c r="F48" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -1869,7 +1898,7 @@
         <v>3.62</v>
       </c>
       <c r="F49" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3345,8 +3374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E3B8CC-8407-8C4C-BFA2-F0515436463B}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3441,7 +3470,7 @@
         <v>4.47</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3461,7 +3490,7 @@
         <v>3.88</v>
       </c>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3472,7 +3501,7 @@
         <v>3.58</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3506,7 +3535,7 @@
         <v>3.33</v>
       </c>
       <c r="F10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -3520,7 +3549,7 @@
         <v>5.04</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -3551,7 +3580,7 @@
         <v>3.98</v>
       </c>
       <c r="F13" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3562,6 +3591,4210 @@
         <v>3.84</v>
       </c>
       <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA41F2D-5A75-4F41-8403-8F85BB70A493}">
+  <dimension ref="A1:F313"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>54.266392999999994</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3.895102820248018</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>54.355229000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3.7949032285143427</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>54.444063999999997</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.6183599291301292</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>54.525214999999996</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3.7684869435164652</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>54.604219999999998</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3.8299814073114056</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>54.683225</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3.5841666367432614</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>54.768633000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3.7260397158832093</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>54.864514</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3.7679864892630808</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>54.915622999999997</v>
+      </c>
+      <c r="E10" s="2">
+        <v>3.8691853987888867</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>54.963121000000001</v>
+      </c>
+      <c r="E11" s="2">
+        <v>3.7178816203790959</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>55.021377999999999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3.8648118714698367</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>55.078666666666699</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3.8818599914211496</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>55.078666666666699</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3.706123536878986</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>55.138220999999994</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3.532042734822463</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>55.138220999999994</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4.0011735646610456</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>55.1967619047619</v>
+      </c>
+      <c r="E17" s="2">
+        <v>3.5177518013638562</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>55.1967619047619</v>
+      </c>
+      <c r="E18" s="2">
+        <v>3.783072589154862</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>55.256582999999999</v>
+      </c>
+      <c r="E19" s="2">
+        <v>3.7489581186202843</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>55.256582999999999</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4.1502178603723188</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>55.376230000000007</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3.5461085126419127</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>55.449718000000004</v>
+      </c>
+      <c r="B22" s="2">
+        <v>15.22</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3.615390103042857</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>55.519707000000004</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="E23" s="2">
+        <v>3.6979768393819183</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>55.54958730158436</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="E24">
+        <v>4.04</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>55.54958730158436</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="E25">
+        <v>3.99</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>55.553079365076421</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="E26">
+        <v>3.83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>55.589483999999999</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="E27" s="2">
+        <v>3.6714856086925676</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>55.606599999997336</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="E28">
+        <v>3.81</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>55.622099999997324</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="E29">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>55.628299999997317</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="E30">
+        <v>4.07</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>55.643799999997299</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="E31">
+        <v>3.82</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>55.648866999999996</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="E32" s="2">
+        <v>3.5136363605028058</v>
+      </c>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>55.659599999997894</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="E33">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>55.673999999997882</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="E34">
+        <v>3.94</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>55.685999999997875</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="E35">
+        <v>3.71</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>55.685999999997875</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="E36">
+        <v>3.71</v>
+      </c>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>55.685999999997875</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="E37">
+        <v>4.21</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>55.697412</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="E38" s="2">
+        <v>3.552465576353776</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>55.697999999997869</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="E39">
+        <v>3.78</v>
+      </c>
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>55.709999999997855</v>
+      </c>
+      <c r="B40" s="2">
+        <v>15.4</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="E40">
+        <v>3.65</v>
+      </c>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>55.712399999997857</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="E41">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>55.714799999997851</v>
+      </c>
+      <c r="B42" s="2">
+        <v>15.39</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>55.733632653059473</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="E43">
+        <v>3.69</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>55.73944897959008</v>
+      </c>
+      <c r="B44" s="2">
+        <v>15.76</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>55.749142857141095</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="E45">
+        <v>3.99</v>
+      </c>
+      <c r="F45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>55.758836734692103</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="E46">
+        <v>3.86</v>
+      </c>
+      <c r="F46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>55.77240816326352</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="E47">
+        <v>4.3</v>
+      </c>
+      <c r="F47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>55.776285714283922</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="E48">
+        <v>3.88</v>
+      </c>
+      <c r="F48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>55.780656999999998</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="E49" s="2">
+        <v>3.5867663522474156</v>
+      </c>
+      <c r="F49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>55.787918367345135</v>
+      </c>
+      <c r="B50" s="2">
+        <v>15.86</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="F50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>55.795673469385946</v>
+      </c>
+      <c r="B51" s="2">
+        <v>15.43</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="E51">
+        <v>4.08</v>
+      </c>
+      <c r="F51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>55.79761224489615</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="E52">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="F52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>55.805367346936954</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="E53">
+        <v>3.46</v>
+      </c>
+      <c r="F53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>55.805367346936954</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="E54">
+        <v>3.71</v>
+      </c>
+      <c r="F54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>55.81506122448797</v>
+      </c>
+      <c r="B55" s="2">
+        <v>15.13</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="F55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>55.820228571425524</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="E56">
+        <v>3.95</v>
+      </c>
+      <c r="F56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>55.821618000000001</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="E57" s="2">
+        <v>3.8907420246448319</v>
+      </c>
+      <c r="F57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>55.8428285714255</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="E58">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="F58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>55.8428285714255</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="E59">
+        <v>4.13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>55.846057142854072</v>
+      </c>
+      <c r="B60" s="2">
+        <v>14.96</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>55.858971428568346</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="E61">
+        <v>4.51</v>
+      </c>
+      <c r="F61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>55.858971428568346</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="E62">
+        <v>4.88</v>
+      </c>
+      <c r="F62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>55.865428571425483</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="E63">
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="F63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>55.868657142854047</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="E64">
+        <v>4.72</v>
+      </c>
+      <c r="F64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>55.868657142854047</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="E65">
+        <v>4.72</v>
+      </c>
+      <c r="F65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>55.87188571428262</v>
+      </c>
+      <c r="B66" s="2">
+        <v>15.09</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="E66">
+        <v>4.79</v>
+      </c>
+      <c r="F66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>55.881571428568321</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="E67">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="F67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>55.881571428568321</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="E68">
+        <v>5.22</v>
+      </c>
+      <c r="F68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>55.885182999999998</v>
+      </c>
+      <c r="B69" s="2">
+        <v>14.9</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E69" s="2">
+        <v>4.4053050743473108</v>
+      </c>
+      <c r="F69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>55.888028571425458</v>
+      </c>
+      <c r="B70" s="2">
+        <v>14.92</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E70">
+        <v>5.01</v>
+      </c>
+      <c r="F70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>55.888028571425458</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="E71">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>55.888028571425458</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="E72">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="F72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>55.894485714282595</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="E73">
+        <v>5.46</v>
+      </c>
+      <c r="F73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>55.900942857139732</v>
+      </c>
+      <c r="B74" s="2">
+        <v>14.46</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="F74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>55.900942857139732</v>
+      </c>
+      <c r="B75" s="2">
+        <v>14.45</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E75">
+        <v>4.83</v>
+      </c>
+      <c r="F75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>55.904171428568304</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="E76">
+        <v>5.28</v>
+      </c>
+      <c r="F76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>55.913857142854006</v>
+      </c>
+      <c r="B77" s="2">
+        <v>15.11</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E77">
+        <v>5.09</v>
+      </c>
+      <c r="F77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>55.923542857139715</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="E78">
+        <v>4.83</v>
+      </c>
+      <c r="F78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>55.923542857139715</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="E79">
+        <v>5.49</v>
+      </c>
+      <c r="F79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>55.926771428568287</v>
+      </c>
+      <c r="B80" s="2">
+        <v>14.82</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E80">
+        <v>5.37</v>
+      </c>
+      <c r="F80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>55.929999999996852</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="E81">
+        <v>5.4</v>
+      </c>
+      <c r="F81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>55.931963963962048</v>
+      </c>
+      <c r="B82" s="2">
+        <v>14.51</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E82">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>55.931963963962048</v>
+      </c>
+      <c r="B83" s="2">
+        <v>14.49</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="E83">
+        <v>5.04</v>
+      </c>
+      <c r="F83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>55.931963963962048</v>
+      </c>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="E84">
+        <v>4.7</v>
+      </c>
+      <c r="F84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>55.933927927926007</v>
+      </c>
+      <c r="B85" s="2">
+        <v>14.76</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>55.941783783781858</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="E86">
+        <v>3.53</v>
+      </c>
+      <c r="F86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>55.943747747745817</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="E87">
+        <v>3.72</v>
+      </c>
+      <c r="F87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>55.945711711709784</v>
+      </c>
+      <c r="B88" s="2">
+        <v>15.35</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E88">
+        <v>3.35</v>
+      </c>
+      <c r="F88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>55.945711711709784</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="E89">
+        <v>3.81</v>
+      </c>
+      <c r="F89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>55.947675675673743</v>
+      </c>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="E90">
+        <v>3.13</v>
+      </c>
+      <c r="F90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>55.947675675673743</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="E91">
+        <v>3.21</v>
+      </c>
+      <c r="F91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>55.947675675673743</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="E92">
+        <v>3.4</v>
+      </c>
+      <c r="F92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>55.949639639637709</v>
+      </c>
+      <c r="B93" s="2">
+        <v>15.73</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="E93">
+        <v>3.33</v>
+      </c>
+      <c r="F93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>55.949639639637709</v>
+      </c>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="E94">
+        <v>3.33</v>
+      </c>
+      <c r="F94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>55.949639639637709</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="E95">
+        <v>3.59</v>
+      </c>
+      <c r="F95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>55.953567567565628</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="E96">
+        <v>3.54</v>
+      </c>
+      <c r="F96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>55.955531531529594</v>
+      </c>
+      <c r="B97" s="2">
+        <v>15.46</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="F97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>55.957495495493554</v>
+      </c>
+      <c r="B98" s="2">
+        <v>15.73</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="E98">
+        <v>3.53</v>
+      </c>
+      <c r="F98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>55.965351351349405</v>
+      </c>
+      <c r="B99" s="2">
+        <v>15.69</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="F99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>55.965351351349405</v>
+      </c>
+      <c r="B100" s="2">
+        <v>15.76</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>55.97124324324129</v>
+      </c>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="E101">
+        <v>3.58</v>
+      </c>
+      <c r="F101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>55.97124324324129</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="E102">
+        <v>3.45</v>
+      </c>
+      <c r="F102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>55.97124324324129</v>
+      </c>
+      <c r="B103" s="2"/>
+      <c r="C103" s="2"/>
+      <c r="E103">
+        <v>4.09</v>
+      </c>
+      <c r="F103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>55.975171171169215</v>
+      </c>
+      <c r="B104" s="2"/>
+      <c r="C104" s="2"/>
+      <c r="E104">
+        <v>3.51</v>
+      </c>
+      <c r="F104" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>55.980796000000005</v>
+      </c>
+      <c r="B105" s="2"/>
+      <c r="C105" s="2"/>
+      <c r="E105" s="2">
+        <v>3.3054483969293984</v>
+      </c>
+      <c r="F105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>55.984990990989026</v>
+      </c>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="E106">
+        <v>3.31</v>
+      </c>
+      <c r="F106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>55.984990990989026</v>
+      </c>
+      <c r="B107" s="2"/>
+      <c r="C107" s="2"/>
+      <c r="E107">
+        <v>3.45</v>
+      </c>
+      <c r="F107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>55.984990990989026</v>
+      </c>
+      <c r="B108" s="2"/>
+      <c r="C108" s="2"/>
+      <c r="E108">
+        <v>3.59</v>
+      </c>
+      <c r="F108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>55.984990990989026</v>
+      </c>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="E109">
+        <v>3.55</v>
+      </c>
+      <c r="F109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>55.984990990989026</v>
+      </c>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+      <c r="E110">
+        <v>3.7</v>
+      </c>
+      <c r="F110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>55.992846846844877</v>
+      </c>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+      <c r="E111">
+        <v>3.53</v>
+      </c>
+      <c r="F111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>56.006987387387383</v>
+      </c>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+      <c r="E112" s="2">
+        <v>3.4665724807241181</v>
+      </c>
+      <c r="F112" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>56.01837837837838</v>
+      </c>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="E113" s="2">
+        <v>3.4083089498782733</v>
+      </c>
+      <c r="F113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>56.020021999999997</v>
+      </c>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="E114" s="2">
+        <v>3.4751338879553675</v>
+      </c>
+      <c r="F114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>56.031929729729733</v>
+      </c>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="E115" s="2">
+        <v>3.3585101297893312</v>
+      </c>
+      <c r="F115" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>56.040963963963961</v>
+      </c>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="E116" s="2">
+        <v>3.1962842834448675</v>
+      </c>
+      <c r="F116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>56.05235495495495</v>
+      </c>
+      <c r="B117" s="2"/>
+      <c r="C117" s="2"/>
+      <c r="E117" s="2">
+        <v>3.3830805488282083</v>
+      </c>
+      <c r="F117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>56.059621621621616</v>
+      </c>
+      <c r="B118" s="2"/>
+      <c r="C118" s="2"/>
+      <c r="E118" s="2">
+        <v>3.3681008990798942</v>
+      </c>
+      <c r="F118" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="1">
+        <v>56.063549549549549</v>
+      </c>
+      <c r="B119" s="2"/>
+      <c r="C119" s="2"/>
+      <c r="E119" s="2">
+        <v>3.4907572995627953</v>
+      </c>
+      <c r="F119" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="1">
+        <v>56.074940540540538</v>
+      </c>
+      <c r="B120" s="2"/>
+      <c r="C120" s="2"/>
+      <c r="E120" s="2">
+        <v>3.3942995872732125</v>
+      </c>
+      <c r="F120" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>56.086331531531528</v>
+      </c>
+      <c r="B121" s="2"/>
+      <c r="C121" s="2"/>
+      <c r="E121" s="2">
+        <v>3.3009272942355663</v>
+      </c>
+      <c r="F121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>56.097526126126127</v>
+      </c>
+      <c r="B122" s="2"/>
+      <c r="C122" s="2"/>
+      <c r="E122" s="2">
+        <v>3.278257036286099</v>
+      </c>
+      <c r="F122" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>56.098900900900901</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="E123" s="2">
+        <v>3.4049996478090385</v>
+      </c>
+      <c r="F123" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>56.108917117117116</v>
+      </c>
+      <c r="B124" s="2"/>
+      <c r="C124" s="2"/>
+      <c r="E124" s="2">
+        <v>3.6732118373422513</v>
+      </c>
+      <c r="F124" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>56.120308108108105</v>
+      </c>
+      <c r="B125" s="2"/>
+      <c r="C125" s="2"/>
+      <c r="E125" s="2">
+        <v>3.6308712838177053</v>
+      </c>
+      <c r="F125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="1">
+        <v>56.120308108108105</v>
+      </c>
+      <c r="B126" s="2">
+        <v>15.26</v>
+      </c>
+      <c r="C126" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="F126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="1">
+        <v>56.120308108108105</v>
+      </c>
+      <c r="B127" s="2">
+        <v>15.34</v>
+      </c>
+      <c r="C127" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="F127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="1">
+        <v>56.120308108108105</v>
+      </c>
+      <c r="B128" s="2">
+        <v>15.37</v>
+      </c>
+      <c r="C128" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="F128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>56.138180180180179</v>
+      </c>
+      <c r="B129" s="2"/>
+      <c r="C129" s="2"/>
+      <c r="E129" s="2">
+        <v>3.3247508353369524</v>
+      </c>
+      <c r="F129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="1">
+        <v>56.196891891891887</v>
+      </c>
+      <c r="B130" s="2"/>
+      <c r="C130" s="2"/>
+      <c r="E130" s="2">
+        <v>3.1187701108728589</v>
+      </c>
+      <c r="F130" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="1">
+        <v>56.262081081081085</v>
+      </c>
+      <c r="B131" s="2"/>
+      <c r="C131" s="2"/>
+      <c r="E131" s="2">
+        <v>3.257630826692453</v>
+      </c>
+      <c r="F131" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="1">
+        <v>56.555432432432433</v>
+      </c>
+      <c r="B132" s="2"/>
+      <c r="C132" s="2"/>
+      <c r="E132" s="2">
+        <v>3.2583749777066551</v>
+      </c>
+      <c r="F132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>56.588027027027024</v>
+      </c>
+      <c r="B133" s="2"/>
+      <c r="C133" s="2"/>
+      <c r="E133" s="2">
+        <v>3.2960367218277318</v>
+      </c>
+      <c r="F133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>56.620621621621623</v>
+      </c>
+      <c r="B134" s="2"/>
+      <c r="C134" s="2"/>
+      <c r="E134" s="2">
+        <v>3.2373338707424693</v>
+      </c>
+      <c r="F134" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="1">
+        <v>56.6858108108108</v>
+      </c>
+      <c r="B135" s="2"/>
+      <c r="C135" s="2"/>
+      <c r="E135" s="2">
+        <v>3.1304656074083637</v>
+      </c>
+      <c r="F135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="1">
+        <v>56.718405405405406</v>
+      </c>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="E136" s="2">
+        <v>3.4822981852969979</v>
+      </c>
+      <c r="F136" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="1">
+        <v>56.786000000000001</v>
+      </c>
+      <c r="B137" s="2"/>
+      <c r="C137" s="2"/>
+      <c r="E137" s="2">
+        <v>3.3154394713731983</v>
+      </c>
+      <c r="F137" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="1">
+        <v>56.856000000000002</v>
+      </c>
+      <c r="B138" s="2"/>
+      <c r="C138" s="2"/>
+      <c r="E138" s="2">
+        <v>3.3916257046586136</v>
+      </c>
+      <c r="F138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="1">
+        <v>56.868183908045978</v>
+      </c>
+      <c r="B139" s="2"/>
+      <c r="C139" s="2"/>
+      <c r="E139" s="2">
+        <v>3.4573430807615164</v>
+      </c>
+      <c r="F139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="1">
+        <v>56.892551724137931</v>
+      </c>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="E140" s="2">
+        <v>3.3251733498093734</v>
+      </c>
+      <c r="F140" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="1">
+        <v>56.904735632183908</v>
+      </c>
+      <c r="B141" s="2"/>
+      <c r="C141" s="2"/>
+      <c r="E141" s="2">
+        <v>3.3258499875679028</v>
+      </c>
+      <c r="F141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="1">
+        <v>56.929103448275868</v>
+      </c>
+      <c r="B142" s="2"/>
+      <c r="C142" s="2"/>
+      <c r="E142" s="2">
+        <v>3.1917216508208526</v>
+      </c>
+      <c r="F142" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="1">
+        <v>56.95347126436782</v>
+      </c>
+      <c r="B143" s="2"/>
+      <c r="C143" s="2"/>
+      <c r="E143" s="2">
+        <v>3.5012316053919768</v>
+      </c>
+      <c r="F143" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="1">
+        <v>57.056822085889571</v>
+      </c>
+      <c r="B144" s="2"/>
+      <c r="C144" s="2"/>
+      <c r="E144" s="2">
+        <v>3.3498697920185707</v>
+      </c>
+      <c r="F144" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="1">
+        <v>57.073754601226995</v>
+      </c>
+      <c r="B145" s="2">
+        <v>16.54</v>
+      </c>
+      <c r="C145" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E145" s="2">
+        <v>3.7684978347834344</v>
+      </c>
+      <c r="F145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="1">
+        <v>57.090687116564418</v>
+      </c>
+      <c r="B146" s="2"/>
+      <c r="C146" s="2"/>
+      <c r="E146" s="2">
+        <v>3.5657371352721592</v>
+      </c>
+      <c r="F146" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="1">
+        <v>57.107619631901848</v>
+      </c>
+      <c r="B147" s="2"/>
+      <c r="C147" s="2"/>
+      <c r="E147" s="2">
+        <v>3.7018245923147082</v>
+      </c>
+      <c r="F147" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="1">
+        <v>57.124552147239264</v>
+      </c>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="E148" s="2">
+        <v>3.411066140672856</v>
+      </c>
+      <c r="F148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="1">
+        <v>57.141484662576687</v>
+      </c>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+      <c r="E149" s="2">
+        <v>3.4619244169475225</v>
+      </c>
+      <c r="F149" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="1">
+        <v>57.15841717791411</v>
+      </c>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
+      <c r="E150" s="2">
+        <v>3.469473505787791</v>
+      </c>
+      <c r="F150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="1">
+        <v>57.175349693251533</v>
+      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+      <c r="E151" s="2">
+        <v>3.4469608647791485</v>
+      </c>
+      <c r="F151" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="1">
+        <v>57.192282208588963</v>
+      </c>
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="E152" s="2">
+        <v>3.6602683380791099</v>
+      </c>
+      <c r="F152" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="1">
+        <v>57.20921472392638</v>
+      </c>
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="E153" s="2">
+        <v>3.6491328625405157</v>
+      </c>
+      <c r="F153" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="1">
+        <v>57.226147239263803</v>
+      </c>
+      <c r="B154" s="2">
+        <v>16.63</v>
+      </c>
+      <c r="C154" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="E154" s="2">
+        <v>3.5792144084532067</v>
+      </c>
+      <c r="F154" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="1">
+        <v>57.242769230769234</v>
+      </c>
+      <c r="B155" s="2"/>
+      <c r="C155" s="2"/>
+      <c r="E155" s="2">
+        <v>3.8157961094265369</v>
+      </c>
+      <c r="F155" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="1">
+        <v>57.258666666666663</v>
+      </c>
+      <c r="B156" s="2"/>
+      <c r="C156" s="2"/>
+      <c r="E156" s="2">
+        <v>3.5792100884564113</v>
+      </c>
+      <c r="F156" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>57.274564102564106</v>
+      </c>
+      <c r="B157" s="2"/>
+      <c r="C157" s="2"/>
+      <c r="E157" s="2">
+        <v>3.4596011456126621</v>
+      </c>
+      <c r="F157" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>57.290461538461543</v>
+      </c>
+      <c r="B158" s="2"/>
+      <c r="C158" s="2"/>
+      <c r="E158" s="2">
+        <v>3.4375060364704133</v>
+      </c>
+      <c r="F158" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>57.322256410256415</v>
+      </c>
+      <c r="B159" s="2"/>
+      <c r="C159" s="2"/>
+      <c r="E159" s="2">
+        <v>3.3931826551376867</v>
+      </c>
+      <c r="F159" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>57.338153846153844</v>
+      </c>
+      <c r="B160" s="2">
+        <v>16.45</v>
+      </c>
+      <c r="C160" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="E160" s="2">
+        <v>3.6741954267815062</v>
+      </c>
+      <c r="F160" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>57.354051282051287</v>
+      </c>
+      <c r="B161" s="2"/>
+      <c r="C161" s="2"/>
+      <c r="E161" s="2">
+        <v>3.6366675275709111</v>
+      </c>
+      <c r="F161" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>57.368592920353983</v>
+      </c>
+      <c r="B162" s="2"/>
+      <c r="C162" s="2"/>
+      <c r="E162" s="2">
+        <v>3.7902268612965937</v>
+      </c>
+      <c r="F162" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>57.381778761061952</v>
+      </c>
+      <c r="B163" s="2"/>
+      <c r="C163" s="2"/>
+      <c r="E163" s="2">
+        <v>3.6448802444908273</v>
+      </c>
+      <c r="F163" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>57.394964601769914</v>
+      </c>
+      <c r="B164" s="2"/>
+      <c r="C164" s="2"/>
+      <c r="E164" s="2">
+        <v>3.5395096641015731</v>
+      </c>
+      <c r="F164" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>57.408150442477876</v>
+      </c>
+      <c r="B165" s="2"/>
+      <c r="C165" s="2"/>
+      <c r="E165" s="2">
+        <v>3.6816108070264546</v>
+      </c>
+      <c r="F165" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>57.421336283185845</v>
+      </c>
+      <c r="B166" s="2"/>
+      <c r="C166" s="2"/>
+      <c r="E166" s="2">
+        <v>3.517743321833017</v>
+      </c>
+      <c r="F166" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>57.434522123893814</v>
+      </c>
+      <c r="B167" s="2"/>
+      <c r="C167" s="2"/>
+      <c r="E167" s="2">
+        <v>3.3504824150386541</v>
+      </c>
+      <c r="F167" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>57.447707964601769</v>
+      </c>
+      <c r="B168" s="2"/>
+      <c r="C168" s="2"/>
+      <c r="E168" s="2">
+        <v>3.3923848234683027</v>
+      </c>
+      <c r="F168" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>57.46089380530973</v>
+      </c>
+      <c r="B169" s="2"/>
+      <c r="C169" s="2"/>
+      <c r="E169" s="2">
+        <v>3.3686710435599765</v>
+      </c>
+      <c r="F169" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>57.474079646017699</v>
+      </c>
+      <c r="B170" s="2"/>
+      <c r="C170" s="2"/>
+      <c r="E170" s="2">
+        <v>3.4427114766106133</v>
+      </c>
+      <c r="F170" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>57.487265486725661</v>
+      </c>
+      <c r="B171" s="2"/>
+      <c r="C171" s="2"/>
+      <c r="E171" s="2">
+        <v>3.5508740203436986</v>
+      </c>
+      <c r="F171" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>57.50045132743363</v>
+      </c>
+      <c r="B172" s="2">
+        <v>16.760000000000002</v>
+      </c>
+      <c r="C172" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E172" s="2">
+        <v>3.382163922617647</v>
+      </c>
+      <c r="F172" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>57.513637168141592</v>
+      </c>
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
+      <c r="E173" s="2">
+        <v>3.5045550728353665</v>
+      </c>
+      <c r="F173" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>57.526823008849554</v>
+      </c>
+      <c r="B174" s="2"/>
+      <c r="C174" s="2"/>
+      <c r="E174" s="2">
+        <v>3.6376450311680215</v>
+      </c>
+      <c r="F174" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>57.540008849557516</v>
+      </c>
+      <c r="B175" s="2"/>
+      <c r="C175" s="2"/>
+      <c r="E175" s="2">
+        <v>3.6329061668021598</v>
+      </c>
+      <c r="F175" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>57.553194690265485</v>
+      </c>
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
+      <c r="E176" s="2">
+        <v>3.7034905629872532</v>
+      </c>
+      <c r="F176" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>57.566380530973447</v>
+      </c>
+      <c r="B177" s="2"/>
+      <c r="C177" s="2"/>
+      <c r="E177" s="2">
+        <v>3.8273056534671097</v>
+      </c>
+      <c r="F177" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>57.579566371681416</v>
+      </c>
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
+      <c r="E178" s="2">
+        <v>3.7081666776552309</v>
+      </c>
+      <c r="F178" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>57.592752212389378</v>
+      </c>
+      <c r="B179" s="2"/>
+      <c r="C179" s="2"/>
+      <c r="E179" s="2">
+        <v>3.4653397466152045</v>
+      </c>
+      <c r="F179" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>57.60593805309734</v>
+      </c>
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
+      <c r="E180" s="2">
+        <v>3.5988835198855242</v>
+      </c>
+      <c r="F180" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" s="1">
+        <v>57.619123893805309</v>
+      </c>
+      <c r="B181" s="2">
+        <v>16.52</v>
+      </c>
+      <c r="C181" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="E181" s="2">
+        <v>3.8892320801578402</v>
+      </c>
+      <c r="F181" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" s="1">
+        <v>57.632309734513271</v>
+      </c>
+      <c r="B182" s="2"/>
+      <c r="C182" s="2"/>
+      <c r="E182" s="2">
+        <v>3.6967632957212135</v>
+      </c>
+      <c r="F182" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" s="1">
+        <v>57.645495575221233</v>
+      </c>
+      <c r="B183" s="2"/>
+      <c r="C183" s="2"/>
+      <c r="E183" s="2">
+        <v>3.7001951276327376</v>
+      </c>
+      <c r="F183" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="1">
+        <v>57.658681415929195</v>
+      </c>
+      <c r="B184" s="2"/>
+      <c r="C184" s="2"/>
+      <c r="E184" s="2">
+        <v>3.6099965058771208</v>
+      </c>
+      <c r="F184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" s="1">
+        <v>57.672594512195118</v>
+      </c>
+      <c r="B185" s="2"/>
+      <c r="C185" s="2"/>
+      <c r="E185" s="2">
+        <v>3.4847000058189548</v>
+      </c>
+      <c r="F185" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" s="1">
+        <v>57.686588414634144</v>
+      </c>
+      <c r="B186" s="2"/>
+      <c r="C186" s="2"/>
+      <c r="E186" s="2">
+        <v>3.5538730324667833</v>
+      </c>
+      <c r="F186" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="1">
+        <v>57.700302439024384</v>
+      </c>
+      <c r="B187" s="2"/>
+      <c r="C187" s="2"/>
+      <c r="E187" s="2">
+        <v>3.5242960031803521</v>
+      </c>
+      <c r="F187" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" s="1">
+        <v>57.707579268292676</v>
+      </c>
+      <c r="B188" s="2"/>
+      <c r="C188" s="2"/>
+      <c r="E188" s="2">
+        <v>3.4102140877273568</v>
+      </c>
+      <c r="F188" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="1">
+        <v>57.721573170731702</v>
+      </c>
+      <c r="B189" s="2"/>
+      <c r="C189" s="2"/>
+      <c r="E189" s="2">
+        <v>3.4875436901785335</v>
+      </c>
+      <c r="F189" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>57.735567073170728</v>
+      </c>
+      <c r="B190" s="2"/>
+      <c r="C190" s="2"/>
+      <c r="E190" s="2">
+        <v>3.4131051496914133</v>
+      </c>
+      <c r="F190" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="1">
+        <v>57.749560975609754</v>
+      </c>
+      <c r="B191" s="2"/>
+      <c r="C191" s="2"/>
+      <c r="E191" s="2">
+        <v>3.4171060184623392</v>
+      </c>
+      <c r="F191" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="1">
+        <v>57.763554878048772</v>
+      </c>
+      <c r="B192" s="2"/>
+      <c r="C192" s="2"/>
+      <c r="E192" s="2">
+        <v>3.3420134668810078</v>
+      </c>
+      <c r="F192" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="1">
+        <v>57.777548780487798</v>
+      </c>
+      <c r="B193" s="2"/>
+      <c r="C193" s="2"/>
+      <c r="E193" s="2">
+        <v>3.378114591117976</v>
+      </c>
+      <c r="F193" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="1">
+        <v>57.791542682926824</v>
+      </c>
+      <c r="B194" s="2"/>
+      <c r="C194" s="2"/>
+      <c r="E194" s="2">
+        <v>3.4873535588301507</v>
+      </c>
+      <c r="F194" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="1">
+        <v>57.80553658536585</v>
+      </c>
+      <c r="B195" s="2">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="C195" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="E195" s="2">
+        <v>3.5172919885967446</v>
+      </c>
+      <c r="F195" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" s="1">
+        <v>57.819530487804876</v>
+      </c>
+      <c r="B196" s="2"/>
+      <c r="C196" s="2"/>
+      <c r="E196" s="2">
+        <v>3.5880456744376765</v>
+      </c>
+      <c r="F196" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" s="1">
+        <v>57.833524390243895</v>
+      </c>
+      <c r="B197" s="2"/>
+      <c r="C197" s="2"/>
+      <c r="E197" s="2">
+        <v>3.7936795281295432</v>
+      </c>
+      <c r="F197" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" s="1">
+        <v>57.847518292682921</v>
+      </c>
+      <c r="B198" s="2"/>
+      <c r="C198" s="2"/>
+      <c r="E198" s="2">
+        <v>3.5693221951681329</v>
+      </c>
+      <c r="F198" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" s="1">
+        <v>57.861512195121946</v>
+      </c>
+      <c r="B199" s="2"/>
+      <c r="C199" s="2"/>
+      <c r="E199" s="2">
+        <v>3.4273006076323909</v>
+      </c>
+      <c r="F199" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A200" s="1">
+        <v>57.875506097560972</v>
+      </c>
+      <c r="B200" s="2"/>
+      <c r="C200" s="2"/>
+      <c r="E200" s="2">
+        <v>3.7062474197487862</v>
+      </c>
+      <c r="F200" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A201" s="1">
+        <v>57.903493902439017</v>
+      </c>
+      <c r="B201" s="2"/>
+      <c r="C201" s="2"/>
+      <c r="E201" s="2">
+        <v>3.6650175377074738</v>
+      </c>
+      <c r="F201" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="1">
+        <v>57.917487804878043</v>
+      </c>
+      <c r="B202" s="2"/>
+      <c r="C202" s="2"/>
+      <c r="E202" s="2">
+        <v>3.7797337974048544</v>
+      </c>
+      <c r="F202" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" s="1">
+        <v>57.931481707317069</v>
+      </c>
+      <c r="B203" s="2"/>
+      <c r="C203" s="2"/>
+      <c r="E203" s="2">
+        <v>3.7878600892900853</v>
+      </c>
+      <c r="F203" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" s="1">
+        <v>57.945475609756095</v>
+      </c>
+      <c r="B204" s="2"/>
+      <c r="C204" s="2"/>
+      <c r="E204" s="2">
+        <v>3.8316205759878095</v>
+      </c>
+      <c r="F204" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A205" s="1">
+        <v>57.95946951219512</v>
+      </c>
+      <c r="B205" s="2"/>
+      <c r="C205" s="2"/>
+      <c r="E205" s="2">
+        <v>3.7137640986938458</v>
+      </c>
+      <c r="F205" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A206" s="1">
+        <v>57.962268292682928</v>
+      </c>
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
+      <c r="E206" s="2">
+        <v>4.0264843288401009</v>
+      </c>
+      <c r="F206" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" s="1">
+        <v>57.973463414634139</v>
+      </c>
+      <c r="B207" s="2"/>
+      <c r="C207" s="2"/>
+      <c r="E207" s="2">
+        <v>3.7667640463586864</v>
+      </c>
+      <c r="F207" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="1">
+        <v>57.976262195121947</v>
+      </c>
+      <c r="B208" s="2"/>
+      <c r="C208" s="2"/>
+      <c r="E208" s="2">
+        <v>3.9007120808267719</v>
+      </c>
+      <c r="F208" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="1">
+        <v>57.987457317073165</v>
+      </c>
+      <c r="B209" s="2">
+        <v>16.47</v>
+      </c>
+      <c r="C209" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="E209" s="2">
+        <v>3.8829780315911004</v>
+      </c>
+      <c r="F209" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="1">
+        <v>57.990256097560973</v>
+      </c>
+      <c r="B210" s="2"/>
+      <c r="C210" s="2"/>
+      <c r="E210" s="2">
+        <v>3.9261288632978486</v>
+      </c>
+      <c r="F210" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="1">
+        <v>58.001451219512191</v>
+      </c>
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
+      <c r="E211" s="2">
+        <v>3.8897362007302734</v>
+      </c>
+      <c r="F211" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="1">
+        <v>58.001451219512191</v>
+      </c>
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="E212" s="2">
+        <v>4.2741134049964771</v>
+      </c>
+      <c r="F212" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="1">
+        <v>58.015445121951217</v>
+      </c>
+      <c r="B213" s="2"/>
+      <c r="C213" s="2"/>
+      <c r="E213" s="2">
+        <v>4.0275865571483553</v>
+      </c>
+      <c r="F213" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" s="1">
+        <v>58.029439024390243</v>
+      </c>
+      <c r="B214" s="2"/>
+      <c r="C214" s="2"/>
+      <c r="E214" s="2">
+        <v>3.9440322611926479</v>
+      </c>
+      <c r="F214" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A215" s="1">
+        <v>58.029439024390243</v>
+      </c>
+      <c r="B215" s="2"/>
+      <c r="C215" s="2"/>
+      <c r="E215" s="2">
+        <v>4.0697313008957092</v>
+      </c>
+      <c r="F215" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A216" s="1">
+        <v>58.043432926829261</v>
+      </c>
+      <c r="B216" s="2"/>
+      <c r="C216" s="2"/>
+      <c r="E216" s="2">
+        <v>3.818651904656075</v>
+      </c>
+      <c r="F216" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217" s="1">
+        <v>58.044832317073173</v>
+      </c>
+      <c r="B217" s="2">
+        <v>16.53</v>
+      </c>
+      <c r="C217" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="E217" s="2">
+        <v>4.3255504982138024</v>
+      </c>
+      <c r="F217" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" s="1">
+        <v>58.057426829268287</v>
+      </c>
+      <c r="B218" s="2"/>
+      <c r="C218" s="2"/>
+      <c r="E218" s="2">
+        <v>4.0091463372134628</v>
+      </c>
+      <c r="F218" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>58.057426829268287</v>
+      </c>
+      <c r="B219" s="2"/>
+      <c r="C219" s="2"/>
+      <c r="E219" s="2">
+        <v>4.3663548244762609</v>
+      </c>
+      <c r="F219" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>58.063707000000001</v>
+      </c>
+      <c r="B220" s="2"/>
+      <c r="C220" s="2"/>
+      <c r="E220" s="2">
+        <v>4.4272088916194727</v>
+      </c>
+      <c r="F220" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221" s="1">
+        <v>58.063707000000001</v>
+      </c>
+      <c r="B221" s="2">
+        <v>16.3</v>
+      </c>
+      <c r="C221" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="E221" s="2">
+        <v>4.3475441586063885</v>
+      </c>
+      <c r="F221" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222" s="1">
+        <v>58.068488000000002</v>
+      </c>
+      <c r="B222" s="2">
+        <v>16.32</v>
+      </c>
+      <c r="C222" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E222" s="2">
+        <v>4.3368171886392846</v>
+      </c>
+      <c r="F222" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A223" s="1">
+        <v>58.068488000000002</v>
+      </c>
+      <c r="B223" s="2"/>
+      <c r="C223" s="2"/>
+      <c r="E223" s="2">
+        <v>4.4749165684706869</v>
+      </c>
+      <c r="F223" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" s="1">
+        <v>58.071420731707313</v>
+      </c>
+      <c r="B224" s="2"/>
+      <c r="C224" s="2"/>
+      <c r="E224" s="2">
+        <v>4.2746468266016837</v>
+      </c>
+      <c r="F224" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A225" s="1">
+        <v>58.072820121951217</v>
+      </c>
+      <c r="B225" s="2"/>
+      <c r="C225" s="2"/>
+      <c r="E225" s="2">
+        <v>4.6187277459150282</v>
+      </c>
+      <c r="F225" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A226" s="1">
+        <v>58.074089000000001</v>
+      </c>
+      <c r="B226" s="2"/>
+      <c r="C226" s="2"/>
+      <c r="E226" s="2">
+        <v>4.2152478442934997</v>
+      </c>
+      <c r="F226" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A227" s="1">
+        <v>58.074089000000001</v>
+      </c>
+      <c r="B227" s="2"/>
+      <c r="C227" s="2"/>
+      <c r="E227" s="2">
+        <v>4.2352746580964524</v>
+      </c>
+      <c r="F227" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
+        <v>58.080834451219502</v>
+      </c>
+      <c r="B228" s="2">
+        <v>15.53</v>
+      </c>
+      <c r="C228" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E228" s="2">
+        <v>4.5685690611454319</v>
+      </c>
+      <c r="F228" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A229" s="1">
+        <v>58.085712000000001</v>
+      </c>
+      <c r="B229" s="2">
+        <v>15.3</v>
+      </c>
+      <c r="C229" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="E229" s="2">
+        <v>4.3313183579238599</v>
+      </c>
+      <c r="F229" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A230" s="1">
+        <v>58.085712000000001</v>
+      </c>
+      <c r="B230" s="2">
+        <v>16.239999999999998</v>
+      </c>
+      <c r="C230" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="E230" s="2">
+        <v>4.4723059787120052</v>
+      </c>
+      <c r="F230" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A231" s="1">
+        <v>58.090893999999999</v>
+      </c>
+      <c r="B231" s="2"/>
+      <c r="C231" s="2"/>
+      <c r="E231" s="2">
+        <v>4.3955521169776244</v>
+      </c>
+      <c r="F231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A232" s="1">
+        <v>58.096494999999997</v>
+      </c>
+      <c r="B232" s="2"/>
+      <c r="C232" s="2"/>
+      <c r="E232" s="2">
+        <v>4.2119135643212706</v>
+      </c>
+      <c r="F232" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A233" s="1">
+        <v>58.099408536585365</v>
+      </c>
+      <c r="B233" s="2">
+        <v>16.22</v>
+      </c>
+      <c r="C233" s="2">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E233" s="2">
+        <v>4.1562997838197067</v>
+      </c>
+      <c r="F233" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
+        <v>58.100807926829262</v>
+      </c>
+      <c r="B234" s="2">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="C234" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E234" s="2">
+        <v>4.397432428373234</v>
+      </c>
+      <c r="F234" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A235" s="1">
+        <v>58.102097000000001</v>
+      </c>
+      <c r="B235" s="2">
+        <v>16.5</v>
+      </c>
+      <c r="C235" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="E235" s="2">
+        <v>4.3702789488753542</v>
+      </c>
+      <c r="F235" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A236" s="1">
+        <v>58.110452195121901</v>
+      </c>
+      <c r="B236" s="2"/>
+      <c r="C236" s="2"/>
+      <c r="E236" s="2">
+        <v>4.3225351414370952</v>
+      </c>
+      <c r="F236" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
+        <v>58.112003048780487</v>
+      </c>
+      <c r="B237" s="2"/>
+      <c r="C237" s="2"/>
+      <c r="E237" s="2">
+        <v>4.2874534453460775</v>
+      </c>
+      <c r="F237" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A238" s="1">
+        <v>58.113402439024384</v>
+      </c>
+      <c r="B238" s="2"/>
+      <c r="C238" s="2"/>
+      <c r="E238" s="2">
+        <v>4.0704837257516591</v>
+      </c>
+      <c r="F238" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A239" s="1">
+        <v>58.116169999999997</v>
+      </c>
+      <c r="B239" s="2"/>
+      <c r="C239" s="2"/>
+      <c r="E239" s="2">
+        <v>4.3332440567396286</v>
+      </c>
+      <c r="F239" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A240" s="1">
+        <v>58.119041000000003</v>
+      </c>
+      <c r="B240" s="2"/>
+      <c r="C240" s="2"/>
+      <c r="E240" s="2">
+        <v>4.165243487209132</v>
+      </c>
+      <c r="F240" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241" s="1">
+        <v>58.127737000000003</v>
+      </c>
+      <c r="B241" s="2"/>
+      <c r="C241" s="2"/>
+      <c r="E241" s="2">
+        <v>4.6430881445686571</v>
+      </c>
+      <c r="F241" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A242" s="1">
+        <v>58.127737000000003</v>
+      </c>
+      <c r="B242" s="2"/>
+      <c r="C242" s="2"/>
+      <c r="E242" s="2">
+        <v>4.310141598477232</v>
+      </c>
+      <c r="F242" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A243" s="1">
+        <v>58.130629213483139</v>
+      </c>
+      <c r="B243" s="2"/>
+      <c r="C243" s="2"/>
+      <c r="E243" s="2">
+        <v>4.0293042876779417</v>
+      </c>
+      <c r="F243" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A244" s="1">
+        <v>58.132567415730335</v>
+      </c>
+      <c r="B244" s="2">
+        <v>16.53</v>
+      </c>
+      <c r="C244" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="E244" s="2">
+        <v>3.9310864587406535</v>
+      </c>
+      <c r="F244" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A245" s="1">
+        <v>58.136240999999998</v>
+      </c>
+      <c r="B245" s="2"/>
+      <c r="C245" s="2"/>
+      <c r="E245" s="2">
+        <v>4.195911897164958</v>
+      </c>
+      <c r="F245" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A246" s="1">
+        <v>58.136240999999998</v>
+      </c>
+      <c r="B246" s="2"/>
+      <c r="C246" s="2"/>
+      <c r="E246" s="2">
+        <v>4.0778653986934499</v>
+      </c>
+      <c r="F246" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>58.149182752808898</v>
+      </c>
+      <c r="B247" s="2"/>
+      <c r="C247" s="2"/>
+      <c r="E247" s="2">
+        <v>4.2368952768146766</v>
+      </c>
+      <c r="F247" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A248" s="1">
+        <v>58.149182752808898</v>
+      </c>
+      <c r="B248" s="2"/>
+      <c r="C248" s="2"/>
+      <c r="E248" s="2">
+        <v>4.2458664663771168</v>
+      </c>
+      <c r="F248" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A249" s="1">
+        <v>58.150011235955056</v>
+      </c>
+      <c r="B249" s="2"/>
+      <c r="C249" s="2"/>
+      <c r="E249" s="2">
+        <v>4.1839018556810874</v>
+      </c>
+      <c r="F249" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A250" s="1">
+        <v>58.153440000000003</v>
+      </c>
+      <c r="B250" s="2"/>
+      <c r="C250" s="2"/>
+      <c r="E250" s="2">
+        <v>4.4263140663950002</v>
+      </c>
+      <c r="F250" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A251" s="1">
+        <v>58.153440000000003</v>
+      </c>
+      <c r="B251" s="2"/>
+      <c r="C251" s="2"/>
+      <c r="E251" s="2">
+        <v>4.2916120171566572</v>
+      </c>
+      <c r="F251" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A252" s="1">
+        <v>58.15388764044944</v>
+      </c>
+      <c r="B252" s="2"/>
+      <c r="C252" s="2"/>
+      <c r="E252" s="2">
+        <v>4.6892398089174083</v>
+      </c>
+      <c r="F252" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A253" s="1">
+        <v>58.162137000000001</v>
+      </c>
+      <c r="B253" s="2"/>
+      <c r="C253" s="2"/>
+      <c r="E253" s="2">
+        <v>4.3588954284302925</v>
+      </c>
+      <c r="F253" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A254" s="1">
+        <v>58.169393258426965</v>
+      </c>
+      <c r="B254" s="2"/>
+      <c r="C254" s="2"/>
+      <c r="E254" s="2">
+        <v>3.9775255300043684</v>
+      </c>
+      <c r="F254" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A255" s="1">
+        <v>58.170833000000002</v>
+      </c>
+      <c r="B255" s="2"/>
+      <c r="C255" s="2"/>
+      <c r="E255" s="2">
+        <v>4.1854519852198138</v>
+      </c>
+      <c r="F255" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A256" s="1">
+        <v>58.173269662921349</v>
+      </c>
+      <c r="B256" s="2"/>
+      <c r="C256" s="2"/>
+      <c r="E256" s="2">
+        <v>4.553475983396055</v>
+      </c>
+      <c r="F256" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A257" s="1">
+        <v>58.179335999999992</v>
+      </c>
+      <c r="B257" s="2"/>
+      <c r="C257" s="2"/>
+      <c r="E257" s="2">
+        <v>4.3666350591807044</v>
+      </c>
+      <c r="F257" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A258" s="1">
+        <v>58.188775280898874</v>
+      </c>
+      <c r="B258" s="2"/>
+      <c r="C258" s="2"/>
+      <c r="E258" s="2">
+        <v>4.0146544843671803</v>
+      </c>
+      <c r="F258" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A259" s="1">
+        <v>58.190713483146062</v>
+      </c>
+      <c r="B259" s="2"/>
+      <c r="C259" s="2"/>
+      <c r="E259" s="2">
+        <v>4.8713971040367205</v>
+      </c>
+      <c r="F259" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A260" s="1">
+        <v>58.190713483146062</v>
+      </c>
+      <c r="B260" s="2"/>
+      <c r="C260" s="2"/>
+      <c r="E260" s="2">
+        <v>4.4660701626620956</v>
+      </c>
+      <c r="F260" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A261" s="1">
+        <v>58.1919550561798</v>
+      </c>
+      <c r="B261" s="2"/>
+      <c r="C261" s="2"/>
+      <c r="E261" s="2">
+        <v>4.1547068454551779</v>
+      </c>
+      <c r="F261" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A262" s="1">
+        <v>58.196536000000002</v>
+      </c>
+      <c r="B262" s="2"/>
+      <c r="C262" s="2"/>
+      <c r="E262" s="2">
+        <v>4.3736122706207494</v>
+      </c>
+      <c r="F262" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A263" s="1">
+        <v>58.201544943820203</v>
+      </c>
+      <c r="B263" s="2"/>
+      <c r="C263" s="2"/>
+      <c r="E263" s="2">
+        <v>4.1039680210376943</v>
+      </c>
+      <c r="F263" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A264" s="1">
+        <v>58.208157303370783</v>
+      </c>
+      <c r="B264" s="2"/>
+      <c r="C264" s="2"/>
+      <c r="E264" s="2">
+        <v>4.0421846975218934</v>
+      </c>
+      <c r="F264" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>58.210095505617971</v>
+      </c>
+      <c r="B265" s="2"/>
+      <c r="C265" s="2"/>
+      <c r="E265" s="2">
+        <v>4.0641753586789928</v>
+      </c>
+      <c r="F265" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A266" s="1">
+        <v>58.218188764044903</v>
+      </c>
+      <c r="B266" s="2"/>
+      <c r="C266" s="2"/>
+      <c r="E266" s="2">
+        <v>3.9880749332152838</v>
+      </c>
+      <c r="F266" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>58.224477528089899</v>
+      </c>
+      <c r="B267" s="2"/>
+      <c r="C267" s="2"/>
+      <c r="E267" s="2">
+        <v>4.0922018766079962</v>
+      </c>
+      <c r="F267" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
+        <v>58.227539325842692</v>
+      </c>
+      <c r="B268" s="2"/>
+      <c r="C268" s="2"/>
+      <c r="E268" s="2">
+        <v>3.8282685361348996</v>
+      </c>
+      <c r="F268" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A269" s="1">
+        <v>58.22947752808988</v>
+      </c>
+      <c r="B269" s="2"/>
+      <c r="C269" s="2"/>
+      <c r="E269" s="2">
+        <v>4.0737761760001421</v>
+      </c>
+      <c r="F269" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A270" s="1">
+        <v>58.235137640449402</v>
+      </c>
+      <c r="B270" s="2"/>
+      <c r="C270" s="2"/>
+      <c r="E270" s="2">
+        <v>4.0234679878589912</v>
+      </c>
+      <c r="F270" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A271" s="1">
+        <v>58.239631000000003</v>
+      </c>
+      <c r="B271" s="2"/>
+      <c r="C271" s="2"/>
+      <c r="E271" s="2">
+        <v>3.7196482134603381</v>
+      </c>
+      <c r="F271" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A272" s="1">
+        <v>58.246921348314608</v>
+      </c>
+      <c r="B272" s="2"/>
+      <c r="C272" s="2"/>
+      <c r="E272" s="2">
+        <v>3.9158535269079255</v>
+      </c>
+      <c r="F272" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A273" s="1">
+        <v>58.248328000000001</v>
+      </c>
+      <c r="B273" s="2"/>
+      <c r="C273" s="2"/>
+      <c r="E273" s="2">
+        <v>3.9497071099329562</v>
+      </c>
+      <c r="F273" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A274" s="1">
+        <v>58.248859550561797</v>
+      </c>
+      <c r="B274" s="2"/>
+      <c r="C274" s="2"/>
+      <c r="E274" s="2">
+        <v>4.3845355152405903</v>
+      </c>
+      <c r="F274" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
+        <v>58.248859550561797</v>
+      </c>
+      <c r="B275" s="2"/>
+      <c r="C275" s="2"/>
+      <c r="E275" s="2">
+        <v>4.0931187480521931</v>
+      </c>
+      <c r="F275" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
+        <v>58.257024000000008</v>
+      </c>
+      <c r="B276" s="2"/>
+      <c r="C276" s="2"/>
+      <c r="E276" s="2">
+        <v>4.0886303688278751</v>
+      </c>
+      <c r="F276" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A277" s="1">
+        <v>58.265526999999999</v>
+      </c>
+      <c r="B277" s="2"/>
+      <c r="C277" s="2"/>
+      <c r="E277" s="2">
+        <v>4.1104126957536815</v>
+      </c>
+      <c r="F277" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A278" s="1">
+        <v>58.266303370786517</v>
+      </c>
+      <c r="B278" s="2"/>
+      <c r="C278" s="2"/>
+      <c r="E278" s="2">
+        <v>3.9839362109614869</v>
+      </c>
+      <c r="F278" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
+        <v>58.268241573033706</v>
+      </c>
+      <c r="B279" s="2"/>
+      <c r="C279" s="2"/>
+      <c r="E279" s="2">
+        <v>4.3866562096999031</v>
+      </c>
+      <c r="F279" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A280" s="1">
+        <v>58.268241573033706</v>
+      </c>
+      <c r="B280" s="2"/>
+      <c r="C280" s="2"/>
+      <c r="E280" s="2">
+        <v>4.1541493231447095</v>
+      </c>
+      <c r="F280" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A281" s="1">
+        <v>58.278531910112399</v>
+      </c>
+      <c r="B281" s="2"/>
+      <c r="C281" s="2"/>
+      <c r="E281" s="2">
+        <v>3.9251802585002973</v>
+      </c>
+      <c r="F281" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
+        <v>58.282727000000001</v>
+      </c>
+      <c r="B282" s="2"/>
+      <c r="C282" s="2"/>
+      <c r="E282" s="2">
+        <v>3.8513743533478522</v>
+      </c>
+      <c r="F282" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A283" s="1">
+        <v>58.285685393258426</v>
+      </c>
+      <c r="B283" s="2">
+        <v>16.39</v>
+      </c>
+      <c r="C283" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E283" s="2">
+        <v>3.8191541607907862</v>
+      </c>
+      <c r="F283" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A284" s="1">
+        <v>58.287623595505622</v>
+      </c>
+      <c r="B284" s="2"/>
+      <c r="C284" s="2"/>
+      <c r="E284" s="2">
+        <v>3.9303295140128958</v>
+      </c>
+      <c r="F284" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
+        <v>58.287623595505622</v>
+      </c>
+      <c r="B285" s="2"/>
+      <c r="C285" s="2"/>
+      <c r="E285" s="2">
+        <v>4.4074986156178424</v>
+      </c>
+      <c r="F285" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
+        <v>58.305067415730335</v>
+      </c>
+      <c r="B286" s="2"/>
+      <c r="C286" s="2"/>
+      <c r="E286" s="2">
+        <v>3.7432312987053131</v>
+      </c>
+      <c r="F286" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
+        <v>58.308943820224719</v>
+      </c>
+      <c r="B287" s="2"/>
+      <c r="C287" s="2"/>
+      <c r="E287" s="2">
+        <v>4.4319520363919889</v>
+      </c>
+      <c r="F287" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A288" s="1">
+        <v>58.308943820224719</v>
+      </c>
+      <c r="B288" s="2"/>
+      <c r="C288" s="2"/>
+      <c r="E288" s="2">
+        <v>4.2238186090390819</v>
+      </c>
+      <c r="F288" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A289" s="1">
+        <v>58.324449438202244</v>
+      </c>
+      <c r="B289" s="2"/>
+      <c r="C289" s="2"/>
+      <c r="E289" s="2">
+        <v>3.8063341193479467</v>
+      </c>
+      <c r="F289" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A290" s="1">
+        <v>58.328325842696628</v>
+      </c>
+      <c r="B290" s="2"/>
+      <c r="C290" s="2"/>
+      <c r="E290" s="2">
+        <v>4.0444948318193319</v>
+      </c>
+      <c r="F290" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A291" s="1">
+        <v>58.343831460674153</v>
+      </c>
+      <c r="B291" s="2"/>
+      <c r="C291" s="2"/>
+      <c r="E291" s="2">
+        <v>3.7991153106936015</v>
+      </c>
+      <c r="F291" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A292" s="1">
+        <v>58.363213483146062</v>
+      </c>
+      <c r="B292" s="2"/>
+      <c r="C292" s="2"/>
+      <c r="E292" s="2">
+        <v>3.6256369657562471</v>
+      </c>
+      <c r="F292" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" s="1">
+        <v>58.382595505617971</v>
+      </c>
+      <c r="B293" s="2"/>
+      <c r="C293" s="2"/>
+      <c r="E293" s="2">
+        <v>3.7318977899146955</v>
+      </c>
+      <c r="F293" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A294" s="1">
+        <v>58.40197752808988</v>
+      </c>
+      <c r="B294" s="2"/>
+      <c r="C294" s="2"/>
+      <c r="E294" s="2">
+        <v>3.8829572681161735</v>
+      </c>
+      <c r="F294" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A295" s="1">
+        <v>58.421359550561789</v>
+      </c>
+      <c r="B295" s="2"/>
+      <c r="C295" s="2"/>
+      <c r="E295" s="2">
+        <v>3.7627552376366307</v>
+      </c>
+      <c r="F295" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A296" s="1">
+        <v>58.440741573033705</v>
+      </c>
+      <c r="B296" s="2">
+        <v>15.95</v>
+      </c>
+      <c r="C296" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="E296" s="2">
+        <v>3.9847466007280676</v>
+      </c>
+      <c r="F296" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A297" s="1">
+        <v>58.460123595505614</v>
+      </c>
+      <c r="B297" s="2"/>
+      <c r="C297" s="2"/>
+      <c r="E297" s="2">
+        <v>3.8353988455911567</v>
+      </c>
+      <c r="F297" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A298" s="1">
+        <v>58.478803738317751</v>
+      </c>
+      <c r="B298" s="2"/>
+      <c r="C298" s="2"/>
+      <c r="E298" s="2">
+        <v>3.5621736227323431</v>
+      </c>
+      <c r="F298" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A299" s="1">
+        <v>58.497308411214945</v>
+      </c>
+      <c r="B299" s="2"/>
+      <c r="C299" s="2"/>
+      <c r="E299" s="2">
+        <v>3.6852993782444652</v>
+      </c>
+      <c r="F299" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A300" s="1">
+        <v>58.515813084112146</v>
+      </c>
+      <c r="B300" s="2"/>
+      <c r="C300" s="2"/>
+      <c r="E300" s="2">
+        <v>3.5963373835282217</v>
+      </c>
+      <c r="F300" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A301" s="1">
+        <v>58.534317757009347</v>
+      </c>
+      <c r="B301" s="2"/>
+      <c r="C301" s="2"/>
+      <c r="E301" s="2">
+        <v>3.5636636701345221</v>
+      </c>
+      <c r="F301" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A302" s="1">
+        <v>58.552822429906541</v>
+      </c>
+      <c r="B302" s="2"/>
+      <c r="C302" s="2"/>
+      <c r="E302" s="2">
+        <v>3.4792328193274642</v>
+      </c>
+      <c r="F302" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A303" s="1">
+        <v>58.571327102803735</v>
+      </c>
+      <c r="B303" s="2"/>
+      <c r="C303" s="2"/>
+      <c r="E303" s="2">
+        <v>3.3879401099512916</v>
+      </c>
+      <c r="F303" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A304" s="1">
+        <v>58.605005607476635</v>
+      </c>
+      <c r="B304" s="2"/>
+      <c r="C304" s="2"/>
+      <c r="E304" s="2">
+        <v>3.4136376897272096</v>
+      </c>
+      <c r="F304" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A305" s="3">
+        <v>58.621474766355142</v>
+      </c>
+      <c r="B305" s="4">
+        <v>16.75</v>
+      </c>
+      <c r="C305" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="E305" s="4">
+        <v>3.4961103868895274</v>
+      </c>
+      <c r="F305" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A306" s="1">
+        <v>58.63775887850467</v>
+      </c>
+      <c r="B306" s="2"/>
+      <c r="C306" s="2"/>
+      <c r="E306" s="2">
+        <v>3.5095977584552749</v>
+      </c>
+      <c r="F306" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A307" s="1">
+        <v>58.654042990654204</v>
+      </c>
+      <c r="B307" s="2"/>
+      <c r="C307" s="2"/>
+      <c r="E307" s="2">
+        <v>3.3877264351492777</v>
+      </c>
+      <c r="F307" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A308" s="1">
+        <v>58.688461682242988</v>
+      </c>
+      <c r="B308" s="2"/>
+      <c r="C308" s="2"/>
+      <c r="E308" s="2">
+        <v>3.3555628595748455</v>
+      </c>
+      <c r="F308" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A309" s="1">
+        <v>58.706041121495325</v>
+      </c>
+      <c r="B309" s="2"/>
+      <c r="C309" s="2"/>
+      <c r="E309" s="2">
+        <v>3.4319398409416784</v>
+      </c>
+      <c r="F309" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A310" s="1">
+        <v>58.723620560747662</v>
+      </c>
+      <c r="B310" s="2"/>
+      <c r="C310" s="2"/>
+      <c r="E310" s="2">
+        <v>3.4576687168943758</v>
+      </c>
+      <c r="F310" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A311" s="1">
+        <v>58.741199999999999</v>
+      </c>
+      <c r="B311" s="2"/>
+      <c r="C311" s="2"/>
+      <c r="E311" s="2">
+        <v>3.7197077765697006</v>
+      </c>
+      <c r="F311" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A312" s="1">
+        <v>58.758779439252336</v>
+      </c>
+      <c r="B312" s="2"/>
+      <c r="C312" s="2"/>
+      <c r="E312" s="2">
+        <v>3.457093500054258</v>
+      </c>
+      <c r="F312" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A313" s="3">
+        <v>58.776358878504674</v>
+      </c>
+      <c r="B313" s="4">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="C313" s="4">
+        <v>0.26</v>
+      </c>
+      <c r="E313" s="4">
+        <v>3.5921559329868713</v>
+      </c>
+      <c r="F313" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>